<commit_message>
sec8lec66, PJ challenge solution
</commit_message>
<xml_diff>
--- a/2018-05-21-Q&AtoKN.xlsx
+++ b/2018-05-21-Q&AtoKN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PJ\Java Projects\Udemy Complete Java Masterclass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PJ\Java Projects\Udemy Complete Java Masterclass\udemycjm\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,9 +35,6 @@
     <t>sec8lec65 konstruktor i super().</t>
   </si>
   <si>
-    <t xml:space="preserve">sec8lec65 czemu switch musi mieć wartość default skoro przeskanowalismy wszystkie wartości? </t>
-  </si>
-  <si>
     <t>Jeżeli mamy metodę, której argumentem jest utworzony typ (nie prymitywny) co oznacza jeżeli zwrócimy null?</t>
   </si>
   <si>
@@ -45,6 +42,9 @@
   </si>
   <si>
     <t>Czy po merge usuwać branche?</t>
+  </si>
+  <si>
+    <t>sec8lec65 czemu switch musi mieć wartość default skoro przeskanowalismy wszystkie wartości? Czy java wie jaki jest pełen zakres danych do sprawdzenia?</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
   <dimension ref="B8:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -414,22 +414,22 @@
     </row>
     <row r="11" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="C11" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="C13" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C14" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sec8lec66, TB challenge solution
</commit_message>
<xml_diff>
--- a/2018-05-21-Q&AtoKN.xlsx
+++ b/2018-05-21-Q&AtoKN.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>@overide to adnotacja, która ma informawać o nadpisaniu metody. Czemu specjalna konstrukcja z @, można by przecież użyć //overide? Czy może to coś więcej niż zwykły komentarz</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>sec8lec65 czemu switch musi mieć wartość default skoro przeskanowalismy wszystkie wartości? Czy java wie jaki jest pełen zakres danych do sprawdzenia?</t>
+  </si>
+  <si>
+    <t>Kiedy używać i co oznacza static?</t>
   </si>
 </sst>
 </file>
@@ -380,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:C14"/>
+  <dimension ref="B8:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -432,6 +435,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="2">
+        <v>43242</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
sec5lec37, min, hours challange
</commit_message>
<xml_diff>
--- a/2018-05-21-Q&AtoKN.xlsx
+++ b/2018-05-21-Q&AtoKN.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>@overide to adnotacja, która ma informawać o nadpisaniu metody. Czemu specjalna konstrukcja z @, można by przecież użyć //overide? Czy może to coś więcej niż zwykły komentarz</t>
   </si>
@@ -57,6 +57,24 @@
   </si>
   <si>
     <t>lec67TB, dlaczego double price = hamburger.itemizeHamburger(); ta metoda się wykonuje? Dlaczego sout na tej metodzie się wykonuje w tej kolejności</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adnotacje sa odczytywane przez srodowiska, frameworki. </t>
+  </si>
+  <si>
+    <t>iterface maja tylko przepisy na metody</t>
+  </si>
+  <si>
+    <t>implementacja</t>
+  </si>
+  <si>
+    <t>late binding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switch random. Tablica trzech ksztaltow. Losuje i wrzycasz trojkat, okrag, kwadrat. </t>
+  </si>
+  <si>
+    <t>overide</t>
   </si>
 </sst>
 </file>
@@ -392,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:C18"/>
+  <dimension ref="B8:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -403,48 +421,65 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="83.28515625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="55.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>43241</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="C12" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>43242</v>
       </c>
@@ -452,7 +487,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C16" s="3" t="s">
         <v>8</v>
       </c>
@@ -468,6 +503,11 @@
     <row r="18" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="C18" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sec19lec293 unit testing with JUnit
</commit_message>
<xml_diff>
--- a/2018-05-21-Q&AtoKN.xlsx
+++ b/2018-05-21-Q&AtoKN.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>@overide to adnotacja, która ma informawać o nadpisaniu metody. Czemu specjalna konstrukcja z @, można by przecież użyć //overide? Czy może to coś więcej niż zwykły komentarz</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>lec70.TB komentarze</t>
+  </si>
+  <si>
+    <t>Można się odwoływać w metodzie Main do innych metod z innych klas instancja.metoda. Jak się można odwołać, nie będąc w metodzie Main do innej klasy?</t>
   </si>
 </sst>
 </file>
@@ -468,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:E33"/>
+  <dimension ref="B8:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -604,6 +607,14 @@
         <v>21</v>
       </c>
     </row>
+    <row r="35" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B35" s="2">
+        <v>43294</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
sec19lec294 unit testing with JUnit
</commit_message>
<xml_diff>
--- a/2018-05-21-Q&AtoKN.xlsx
+++ b/2018-05-21-Q&AtoKN.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>@overide to adnotacja, która ma informawać o nadpisaniu metody. Czemu specjalna konstrukcja z @, można by przecież użyć //overide? Czy może to coś więcej niż zwykły komentarz</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>Można się odwoływać w metodzie Main do innych metod z innych klas instancja.metoda. Jak się można odwołać, nie będąc w metodzie Main do innej klasy?</t>
+  </si>
+  <si>
+    <t>Można utworzyć instancję klasy Klasa nazwa = new Klasa(), lub private Klasa nazwa. Jaka różnica</t>
+  </si>
+  <si>
+    <t>lec67test komentarz</t>
+  </si>
+  <si>
+    <t>lec80 main, jak przetestowac metodę readIntegers. Wejscie rozmiar tablicy, uzytkownik podaje inty a na wyjsciu tablica int[]</t>
   </si>
 </sst>
 </file>
@@ -471,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:E35"/>
+  <dimension ref="B8:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -615,6 +624,21 @@
         <v>22</v>
       </c>
     </row>
+    <row r="36" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C36" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C39" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
sec9lec85 Arraylist challange part1
</commit_message>
<xml_diff>
--- a/2018-05-21-Q&AtoKN.xlsx
+++ b/2018-05-21-Q&AtoKN.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>@overide to adnotacja, która ma informawać o nadpisaniu metody. Czemu specjalna konstrukcja z @, można by przecież użyć //overide? Czy może to coś więcej niż zwykły komentarz</t>
   </si>
@@ -92,9 +92,6 @@
     <t>lec70.TB komentarze</t>
   </si>
   <si>
-    <t>Można się odwoływać w metodzie Main do innych metod z innych klas instancja.metoda. Jak się można odwołać, nie będąc w metodzie Main do innej klasy?</t>
-  </si>
-  <si>
     <t>Można utworzyć instancję klasy Klasa nazwa = new Klasa(), lub private Klasa nazwa. Jaka różnica</t>
   </si>
   <si>
@@ -105,6 +102,18 @@
   </si>
   <si>
     <t>lec81 jak powinno się odwolywac do metod z innego pakkietu. Moje utils</t>
+  </si>
+  <si>
+    <t>lec80, co jest bardziej czasochlonne for do polowy rozmiaru tablicy ale dodatkowa linijka kodu czy krotszy kod ale for po calej tablicy</t>
+  </si>
+  <si>
+    <t>Można się odwoływać w metodzie Main do innych metod z innych klas instancja.metoda. Jak się można odwołać, nie będąc w metodzie Main do innej klasy? - ogólnie jak najlepiej się odwolywac do  metod z innych klas czy pakietów.</t>
+  </si>
+  <si>
+    <t>scanner.nextLine() - "to clear the input buffer' ? Po co jest ta komenda?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lec82 Main. </t>
   </si>
 </sst>
 </file>
@@ -483,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:E40"/>
+  <dimension ref="B8:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -619,32 +628,50 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B35" s="2">
         <v>43294</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="C36" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C38" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="C39" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C40" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C41" s="3" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C42" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B43" s="2">
+        <v>43295</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>